<commit_message>
Fix: Errors in user management
</commit_message>
<xml_diff>
--- a/testdata/vulns.xlsx
+++ b/testdata/vulns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flake/sources/misc/secman/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9543AF4-1C56-D24A-844F-D0A4D747C980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D17244A-9D95-F143-A4DA-BAEF2C9F721C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{020683E2-7424-3846-B1AB-2BE7F429EFC8}"/>
+    <workbookView xWindow="3260" yWindow="2160" windowWidth="31300" windowHeight="17440" xr2:uid="{020683E2-7424-3846-B1AB-2BE7F429EFC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Hostname</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>58 days</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>10.10.10.10</t>
+  </si>
+  <si>
+    <t>TESTDOMAINE</t>
   </si>
 </sst>
 </file>
@@ -137,9 +146,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,13 +485,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD6066B-EA4D-0243-916B-4838DD809F02}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="8" max="8" width="16.1640625" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -492,7 +511,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -528,7 +547,7 @@
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
         <v>14</v>
@@ -550,6 +569,61 @@
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3">
+        <v>888888888888</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="3">
+        <v>888888888888</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>